<commit_message>
Add I2C module, and start defining the state machine for I2C processing.
Add the I2C clock rate register value to the calculation sheet.
</commit_message>
<xml_diff>
--- a/Doc/BaudCalculation.xlsx
+++ b/Doc/BaudCalculation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>F_CPU</t>
   </si>
@@ -39,15 +39,50 @@
   </si>
   <si>
     <t>ERR_PROMILLE</t>
+  </si>
+  <si>
+    <t>USART calculation</t>
+  </si>
+  <si>
+    <t>I2C calculation</t>
+  </si>
+  <si>
+    <t>Prescaler TWPS</t>
+  </si>
+  <si>
+    <t>TWI Bit rate register TWBR</t>
+  </si>
+  <si>
+    <t>SCL frequency</t>
+  </si>
+  <si>
+    <t>set SCL frequency</t>
+  </si>
+  <si>
+    <t>set prescaler</t>
+  </si>
+  <si>
+    <t>result TWI bit rate register value</t>
+  </si>
+  <si>
+    <t>actual SCR frequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -74,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:E6"/>
+  <dimension ref="C1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,7 +404,12 @@
     <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -376,7 +417,7 @@
         <v>9216000</v>
       </c>
     </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -384,7 +425,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -393,7 +434,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -402,13 +443,85 @@
         <v>9600000</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6">
         <f xml:space="preserve"> (E5)/(E3)</f>
         <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>9216000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f xml:space="preserve"> E11 / (16 + (2*E13*(POWER(4,E12))))</f>
+        <v>98042.553191489365</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <f>FLOOR(((E11/E16)-15)/2,1)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <f xml:space="preserve"> E11 / (16 + (2*E18*(POWER(4,E17))))</f>
+        <v>100173.91304347826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>